<commit_message>
Updated test cases with preconditions and post test conditions
</commit_message>
<xml_diff>
--- a/Language and Skills Test Cases..xlsx
+++ b/Language and Skills Test Cases..xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="300">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -19,6 +19,9 @@
     <t>Test Cases</t>
   </si>
   <si>
+    <t>Preconditions</t>
+  </si>
+  <si>
     <t>Test Steps</t>
   </si>
   <si>
@@ -31,16 +34,25 @@
     <t>Test Status</t>
   </si>
   <si>
+    <t>Post Test Conditions</t>
+  </si>
+  <si>
     <t>TC_001</t>
   </si>
   <si>
     <t>Verify that an existing user can sign in with valid credentials.</t>
+  </si>
+  <si>
+    <t>1.Ensure there is an existing user account in the system
+with known credentials.
+2.Ensure user account is active.
+3.Ensure the sign in page is functioning properly.</t>
   </si>
   <si>
     <t>1.Navigate to the website.
 2.Click on the Sign-in button.
-3.Enter valid email address.
-4.Enter valid password.
+3.Enter valid email address.(test123@test.com)
+4.Enter valid password.(test123)
 5.Click on the login button.</t>
   </si>
   <si>
@@ -53,18 +65,53 @@
     <t>PASS</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <rFont val="Söhne, ui-sans-serif, system-ui, -apple-system, &quot;Segoe UI&quot;, Roboto, Ubuntu, Cantarell, &quot;Noto Sans&quot;, sans-serif, &quot;Helvetica Neue&quot;, Arial, &quot;Apple Color Emoji&quot;, &quot;Segoe UI Emoji&quot;, &quot;Segoe UI Symbol&quot;, &quot;Noto Color Emoji&quot;"/>
+        <color rgb="FF0D0D0D"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">1.Navigate to the sign-out option.
+2.Click the "Sign Out" button.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Söhne, ui-sans-serif, system-ui, -apple-system, &quot;Segoe UI&quot;, Roboto, Ubuntu, Cantarell, &quot;Noto Sans&quot;, sans-serif, &quot;Helvetica Neue&quot;, Arial, &quot;Apple Color Emoji&quot;, &quot;Segoe UI Emoji&quot;, &quot;Segoe UI Symbol&quot;, &quot;Noto Color Emoji&quot;"/>
+        <color rgb="FF0D0D0D"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Söhne, ui-sans-serif, system-ui, -apple-system, &quot;Segoe UI&quot;, Roboto, Ubuntu, Cantarell, &quot;Noto Sans&quot;, sans-serif, &quot;Helvetica Neue&quot;, Arial, &quot;Apple Color Emoji&quot;, &quot;Segoe UI Emoji&quot;, &quot;Segoe UI Symbol&quot;, &quot;Noto Color Emoji&quot;"/>
+        <color rgb="FF0D0D0D"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">Ensure any test data related to sign in is 
+cleared. </t>
+    </r>
+  </si>
+  <si>
     <t>TC_002</t>
   </si>
   <si>
     <t>Verify that a new user can join with valid details.</t>
   </si>
   <si>
+    <t xml:space="preserve">1.Ensure the registration page is functioning properly.
+2.Ensure that there is no existing user in the system with the
+same details.
+</t>
+  </si>
+  <si>
     <t>1.Click on the Join button.
-2.Enter a valid first name.
-3.Enter a valid last name.
-4.Enter a valid email address.
-5.Enter a valid password.
-6.Confirm password.
+2.Enter a valid first name.(John)
+3.Enter a valid last name.(Miller)
+4.Enter a valid email address.(test1234@gmail.com)
+5.Enter a valid password.(test1234)
+6.Confirm password.(test1234)
 7.Check box the terms and conditions.
 8.Click on join button.</t>
   </si>
@@ -75,10 +122,23 @@
     <t>The user created an account successfully.</t>
   </si>
   <si>
+    <t xml:space="preserve">1.Ensure the user has successfully joined.
+2.Verify that the user's name or profile
+information is displayed.
+3.Ensure any test data related to the test is 
+cleared. 
+</t>
+  </si>
+  <si>
     <t>TC_003</t>
   </si>
   <si>
     <t>Verify that user can add a new language.</t>
+  </si>
+  <si>
+    <t>1.User is already logged in.
+2.Ensure that the user can access Languages section.
+3.Delete all existing languages.</t>
   </si>
   <si>
     <t>1.Navigate and select languages.
@@ -96,10 +156,21 @@
 language is added to the list successfully.</t>
   </si>
   <si>
+    <t>1.Find and remove the new language
+(eg.,English) from the list.
+2.Confirm deletion.
+3.Click on 'Sign out'.</t>
+  </si>
+  <si>
     <t>TC_004</t>
   </si>
   <si>
     <t>Verify that user can add a new skill.</t>
+  </si>
+  <si>
+    <t>1.User is already logged in.
+2.Ensure that the user can access Skills section.
+3.Delete all existing skills.</t>
   </si>
   <si>
     <t>1.Navigate and select skills.
@@ -117,11 +188,22 @@
 is added to the list successfully.</t>
   </si>
   <si>
+    <t>1.Find and remove the new skill
+(eg.,Test Analyst) from the list.
+2.Confirm deletion.
+3.Click on 'Sign out'.</t>
+  </si>
+  <si>
     <t>TC_005</t>
   </si>
   <si>
     <t>Verify that user can not join with an email address
 that is already in use.</t>
+  </si>
+  <si>
+    <t>1.Ensure that there is an existing user in the system with the
+same email address.(test123@test.com).
+2.Ensure that the registration page functioning properly.</t>
   </si>
   <si>
     <t>1.Click on Join button.
@@ -139,6 +221,12 @@
 that the email address already exist.</t>
   </si>
   <si>
+    <t>1.Verify that no new user account was created
+with the email that already exist
+(test123@test.com).
+2. Clear test data.</t>
+  </si>
+  <si>
     <t>TC_006</t>
   </si>
   <si>
@@ -146,8 +234,13 @@
 but an invalid password.</t>
   </si>
   <si>
+    <t>1.Ensure there is an existing user account in the 
+system with known credentials.(test123@test.com,test123)
+2.Ensure that the sign in page is functioning properly.</t>
+  </si>
+  <si>
     <t>1.Navigate to the login page.
-2.Enter valid email id and incorrect password.
+2.Enter valid email id(test123@test.com) and incorrect password.(test567).
 3.Click Login.</t>
   </si>
   <si>
@@ -159,6 +252,11 @@
 'Email verification sent'.</t>
   </si>
   <si>
+    <t>1.Verify that the user is not logged in and
+remains on the sign-in page.
+2.Ensure test data is cleared.</t>
+  </si>
+  <si>
     <t>TC_007</t>
   </si>
   <si>
@@ -166,8 +264,13 @@
 but an invalid email.</t>
   </si>
   <si>
+    <t>1.Ensure there is an existing user account in the 
+system with known credentials.(test123@test.com,test123)
+2.Ensure that the sign in page is functioning properly.</t>
+  </si>
+  <si>
     <t>1.Navigate to the login page.
-2.Enter invalid email id and correct password.
+2.Enter invalid email id(test111@test.com) and correct password(test123).
 3.Click Login.</t>
   </si>
   <si>
@@ -179,11 +282,20 @@
 'Email verification sent'.</t>
   </si>
   <si>
+    <t>1.Verify that the user is not logged in and
+remains on the sign-in page.
+2.Ensure test data is cleared.</t>
+  </si>
+  <si>
     <t>TC_008</t>
   </si>
   <si>
     <t>Verify that user can not join by leaving either first and last name
 or both fields empty.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Ensure the registration page is working properly.
+</t>
   </si>
   <si>
     <t>1.Navigate to account registration page.
@@ -200,10 +312,20 @@
 is a required field and is not able to join.</t>
   </si>
   <si>
+    <t xml:space="preserve">1.Ensure that the registration process is halted
+and the user is not created.
+2.Ensure test data is cleared.
+</t>
+  </si>
+  <si>
     <t>TC_009</t>
   </si>
   <si>
     <t>Verify that the user cannot join without agreeing to the terms and conditions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Ensure the registration page is working properly.
+</t>
   </si>
   <si>
     <t>1.Navigate to account registration page.
@@ -218,6 +340,11 @@
     <t>The user could not click on the Join button.</t>
   </si>
   <si>
+    <t>1.Ensure that the registration process is halted
+and the user is not created.
+2.Ensure test data is cleared.</t>
+  </si>
+  <si>
     <t>TC_010</t>
   </si>
   <si>
@@ -225,8 +352,12 @@
 level.</t>
   </si>
   <si>
+    <t>1.User is already logged in with valid email(test123@test.co
+m)and password(test123).</t>
+  </si>
+  <si>
     <t>1.Navigate to languages and click on Add new button.
-2.Enter language.
+2.Enter language.(eg.,Spanish)
 3.Click on Add button.</t>
   </si>
   <si>
@@ -240,10 +371,20 @@
 language is not added.</t>
   </si>
   <si>
+    <t>1.Ensure 'Spanish' is not added to the list.
+2.Navigate to Sign out and Click on 'Sign out'
+button.</t>
+  </si>
+  <si>
     <t>TC_011</t>
   </si>
   <si>
     <t>Verify that the user cannot add a language without entering the language name.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.User is already logged in with valid email(test123@test.co
+m)and password(test123).
+</t>
   </si>
   <si>
     <t>1.Navigate to languages and click on Add new button.
@@ -261,6 +402,11 @@
 language is not added.</t>
   </si>
   <si>
+    <t>1.Ensure language is not added to the list.
+2.Navigate to Sign out and Click on 'Sign out'
+button.</t>
+  </si>
+  <si>
     <t>TC_012</t>
   </si>
   <si>
@@ -268,8 +414,13 @@
 a language level which already exists.</t>
   </si>
   <si>
+    <t>1.User is already logged in with valid email(test123@test.co
+m)and password(test123).
+2.A Language (eg., Spanish) already exists in the list.</t>
+  </si>
+  <si>
     <t>1.Navigate to languages and click on Add new button.
-2.Enter a language and choose a language level that already exist.
+2.Enter a language(Spanish) and choose a language level that already exist.
 3.Click on Add button.</t>
   </si>
   <si>
@@ -281,6 +432,11 @@
 that the language already exist in the list.</t>
   </si>
   <si>
+    <t>1.Ensure language is not added twice to the list.
+2.Navigate to Sign out and Click on 'Sign out'
+button.</t>
+  </si>
+  <si>
     <t>TC_013</t>
   </si>
   <si>
@@ -288,9 +444,15 @@
 different language level.</t>
   </si>
   <si>
+    <t>1.User is already logged in with valid email(test123@test.co
+m)and password(test123).
+2.A Language (eg., Spanish) and level(Basic) already
+ exists in the list.</t>
+  </si>
+  <si>
     <t>1.Navigate to languages and click on Add new button.
 2.Enter a language which already exists and
- choose a different language level.
+ choose a different language level.(eg.,Spanish and level-Fluent)
 3.Click on Add button.</t>
   </si>
   <si>
@@ -310,6 +472,10 @@
     <t>Verify that the user cannot add more than 4 languages.</t>
   </si>
   <si>
+    <t>1.User is already logged in with valid email(test123@test.co
+m)and password(test123).</t>
+  </si>
+  <si>
     <t>1.Navigate to languages and click on Add new button.
 2.Choose 4 different languages and language level.
 3.Click on Add button.</t>
@@ -324,10 +490,21 @@
 after adding 4 languages.</t>
   </si>
   <si>
+    <t>1.Ensure 5th language is not added to the list.
+2.Navigate to Sign out and Click on 'Sign out'
+button.
+3.Delete test data.</t>
+  </si>
+  <si>
     <t>TC_015</t>
   </si>
   <si>
     <t>Verify that the user can login with a password which has exactly 6 characters.</t>
+  </si>
+  <si>
+    <t>1.Ensure there is an existing user in the system with a
+password that is exactly 6 characters long. 
+2.Ensure sign in page is working properly.</t>
   </si>
   <si>
     <t>1.Navigate to login or sign in page.
@@ -344,10 +521,20 @@
 successfully.</t>
   </si>
   <si>
+    <t>1.Navigate to Sign out and click on 'Sign out'
+button.
+2.Clear test data.</t>
+  </si>
+  <si>
     <t>TC_016</t>
   </si>
   <si>
     <t>Verify that the system accepts a password with more than 6 characters.</t>
+  </si>
+  <si>
+    <t>1.Ensure there is an existing user in the system with a
+password that is more that 6 characters long. 
+2.Ensure sign in page is working properly.</t>
   </si>
   <si>
     <t>1.Navigate to login or sign in page.
@@ -364,10 +551,19 @@
 successfully.</t>
   </si>
   <si>
+    <t>1.Navigate to Sign out and click on 'Sign out'
+button.
+2.Clear test data.</t>
+  </si>
+  <si>
     <t>TC_017</t>
   </si>
   <si>
     <t>Verify that the system rejects a password with less than 6 characters.</t>
+  </si>
+  <si>
+    <t>1.Ensure the user can access the website.
+2.Ensure all other details are valid.</t>
   </si>
   <si>
     <t>1.Navigate to login or sign in page.
@@ -386,10 +582,19 @@
 error message.</t>
   </si>
   <si>
+    <t xml:space="preserve">1.Ensure account is not created or user is logged
+in.
+</t>
+  </si>
+  <si>
     <t>TC_018</t>
   </si>
   <si>
     <t>Verify that the system rejects an empty password field.</t>
+  </si>
+  <si>
+    <t>1.Ensure the user can access the sign inpage.
+2.Ensure all other details are valid.</t>
   </si>
   <si>
     <t>1.Navigate to login or sign in page.
@@ -407,6 +612,10 @@
 error message.</t>
   </si>
   <si>
+    <t>1.Ensure account is not created or user is logged
+in.</t>
+  </si>
+  <si>
     <t>TC_019</t>
   </si>
   <si>
@@ -429,6 +638,10 @@
  and the skill is not added to the list.</t>
   </si>
   <si>
+    <t>1.Ensure the skill is not added to the list.
+2.Clear all test data.</t>
+  </si>
+  <si>
     <t>TC_020</t>
   </si>
   <si>
@@ -457,8 +670,14 @@
 a skill level which already exists.</t>
   </si>
   <si>
+    <t>1.User is already logged in.
+2.A skill(Test Analyst) and experiance level(Beginner)
+already exists.</t>
+  </si>
+  <si>
     <t>1.Navigate to Skills and click on Add new.
-2.Enter the skill name and choose skill leve which already existsl.
+2.Enter the skill name and choose skill level which already exists.(eg.,Test
+Analyst and level Beginner).
 3.Click on Add.</t>
   </si>
   <si>
@@ -472,6 +691,10 @@
 is not added to the list.</t>
   </si>
   <si>
+    <t>1.Ensure the skill is not added twice to the list.
+2.Clear all test data.</t>
+  </si>
+  <si>
     <t>TC_022</t>
   </si>
   <si>
@@ -480,9 +703,13 @@
 </t>
   </si>
   <si>
+    <t>1.User is already logged in.
+2.Add a language (eg.,French) and choose level(Basic).</t>
+  </si>
+  <si>
     <t>1.Navigate to the Languages section.
-2.Click on the Edit button near already existing language.
-3.Change the language name or proficiency level.
+2.Click on the Edit button near already existing language that is French. 
+3.Change the language name(eg.,Hindi) or proficiency level(eg.,Fluent).
 4.Click on Update.</t>
   </si>
   <si>
@@ -494,10 +721,20 @@
 proficiency level in the user's profile.</t>
   </si>
   <si>
+    <t>1.Ensure Hindi is added to the list.
+2.Navigate to Sign out and click 'sign out'
+button.
+3.Clear all test data.</t>
+  </si>
+  <si>
     <t>TC_023</t>
   </si>
   <si>
     <t>Verify that the system allows the user to delete an existing language.</t>
+  </si>
+  <si>
+    <t>1.User is already logged in.
+2.Add a language (eg.,Spanish) and choose level(Basic).</t>
   </si>
   <si>
     <t>1.Navigate to the Languages section.
@@ -513,6 +750,12 @@
     <t>The language is removed from the list.</t>
   </si>
   <si>
+    <t>1.Ensure "Spanish" is not in the list.
+2.Navigate to Sign out and click 'sign out'
+button.
+3.Clear all test data.</t>
+  </si>
+  <si>
     <t>TC_024</t>
   </si>
   <si>
@@ -520,10 +763,14 @@
 experience level.</t>
   </si>
   <si>
+    <t>1.User is already logged in.
+2.Add a skill (eg.,Testing) and choose level(Beginner).</t>
+  </si>
+  <si>
     <t>1.Navigate to the skills section.
-2.Locate the existing skill (e.g., "Software Testing").
+2.Locate the existing skill (e.g., "Testing").
 3.Click the "Edit" button next to the skill.
-4.Change the skill name or proficiency level.
+4.Change the skill name(Logo Designer) or proficiency level(Intermediate).
 5.Click "Update".</t>
   </si>
   <si>
@@ -535,14 +782,26 @@
 experiance level in the user's profile.</t>
   </si>
   <si>
+    <t xml:space="preserve">1.Ensure "Logo Designer" is added to the list.
+2.Navigate to Sign out and click 'sign out'
+button.
+3.Clear all test data.
+</t>
+  </si>
+  <si>
     <t>TC_025</t>
   </si>
   <si>
     <t>Verify that the system allows the user to delete an existing Skill.</t>
   </si>
   <si>
+    <t>1.User is already logged in.
+2.Add a skill (eg.,Software Testing) and choose
+level(Beginner).</t>
+  </si>
+  <si>
     <t>1.Navigate to the skills section.
-2.Locate the existing skill. (e.g., "Spanish").
+2.Locate the existing skill. (e.g., "Software Testing").
 3.Click the "Delete" button next to the skill.
 4.Confirm the deletion if prompted.</t>
   </si>
@@ -554,11 +813,23 @@
     <t>The skill is removed from the list.</t>
   </si>
   <si>
+    <t>1.Ensure "Software Testing" is not in the list.
+2.Navigate to Sign out and click 'sign out'
+button.
+3.Clear all test data.</t>
+  </si>
+  <si>
     <t>TC_026</t>
   </si>
   <si>
     <t>Verify that the system does not allow the user to save an 
 edited language with empty fields.</t>
+  </si>
+  <si>
+    <t>1.User is already logged in.
+2.User can access the languages section.
+3.Ensure there is atleast one language already added to the 
+list.</t>
   </si>
   <si>
     <t>1.Navigate to the Languages section.
@@ -578,11 +849,24 @@
 its proficiency level.</t>
   </si>
   <si>
+    <t>1.Verify that the language Spanish is not updated
+with empty fields and remains unchanged.
+2.Ensure that the language 'Spanish' still 
+appears unchanged in the list.
+3.Clear all test data.</t>
+  </si>
+  <si>
     <t>TC_027</t>
   </si>
   <si>
     <t>Verify that the system does not allow the user to save an
 edited skill with invalid data.</t>
+  </si>
+  <si>
+    <t>1.User is already logged in.
+2.User can access the skills section.
+3.Ensure there is atleast one skill already added to the 
+list.</t>
   </si>
   <si>
     <t>1.Navigate to the Skills section.
@@ -630,6 +914,11 @@
     <t>Verify that the system does not allow an user to add a language with invalid data.</t>
   </si>
   <si>
+    <t>1.User is already logged in.
+2.Ensure that the user can access languages section.
+3.Delete all existing languages</t>
+  </si>
+  <si>
     <t>1.Navigate to the Languages section.
 2.Click on "Add New".
 3.Enter languages name with invalid data.(eg.,enter special characters
@@ -646,6 +935,12 @@
   <si>
     <t>Verify that the system does not allow the user to save an
 edited language with invalid data.</t>
+  </si>
+  <si>
+    <t>1.User is already logged in.
+2.User can access the languages section.
+3.Ensure there is atleast one language already added to the 
+list.</t>
   </si>
   <si>
     <t>1.Navigate to the Languages section.
@@ -671,8 +966,13 @@
 not leaving the mandotory fields empty.</t>
   </si>
   <si>
+    <t>1.User is already logged in.
+2.User can access the skill sharing page.
+3.Delete all existing skills.</t>
+  </si>
+  <si>
     <t>1.Navigate to the skill sharing page.
-2.Enter a valid title.
+2.Enter a valid title.(eg.,Test Analyst)
 3.Fill in any other mandatory fields required by the form.
 4.Click "Save".</t>
   </si>
@@ -687,11 +987,24 @@
 the skill has been shared successfully.</t>
   </si>
   <si>
+    <t>1.Verify that the shared skill "Test Analyst" 
+appears iin the "Manage Listings" section.
+2.Verify that the shared skill "Test Analyst"
+appears when attemting to search.
+3.Navigate to Sign out and click on 'Sign out'
+button.
+4.Clear test data.</t>
+  </si>
+  <si>
     <t>TC_032</t>
   </si>
   <si>
     <t>Verify that the system does not allow the user to share a skill if
  mandatory fields are left empty.</t>
+  </si>
+  <si>
+    <t>1.User is already logged in.
+2.User can access the skill sharing page.</t>
   </si>
   <si>
     <t>1.Navigate to the skill sharing page.
@@ -708,10 +1021,21 @@
 indicating to fill the form correctly.</t>
   </si>
   <si>
+    <t>1.Verify that the skill with empty title is not added.
+2.Navigate to Sign out and click on 'Sign out'
+button.
+3.Clear test data.</t>
+  </si>
+  <si>
     <t>TC_033</t>
   </si>
   <si>
     <t>Verify that the system rejects special characters at any place in the title.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.User is already logged in.
+2.User can access the skill sharing page.
+</t>
   </si>
   <si>
     <t>1.Navigate to the skill sharing page.
@@ -731,6 +1055,13 @@
 </t>
   </si>
   <si>
+    <t>1.Verify that title with special characters
+is not added.
+2.Navigate to Sign out and click on 'Sign out'
+button.
+3.Clear test data.</t>
+  </si>
+  <si>
     <t>TC_034</t>
   </si>
   <si>
@@ -754,10 +1085,22 @@
  an alphabet character or a number.</t>
   </si>
   <si>
+    <t>1.Verify that title with space
+is not added.
+2.Navigate to Sign out and click on 'Sign out'
+button.
+3.Clear test data.</t>
+  </si>
+  <si>
     <t>TC_035</t>
   </si>
   <si>
     <t>Verify that the system rejects special characters at any place in the description.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.User is already logged in.
+2.User can access the skill sharing page.
+</t>
   </si>
   <si>
     <t>1.Navigate to the skill sharing page.
@@ -777,6 +1120,13 @@
 allowed.</t>
   </si>
   <si>
+    <t>1.Verify that description with special characters
+is not added.
+2.Navigate to Sign out and click on 'Sign out'
+button.
+3.Clear test data.</t>
+  </si>
+  <si>
     <t>TC_036</t>
   </si>
   <si>
@@ -800,10 +1150,21 @@
  an alphabet character or a number.</t>
   </si>
   <si>
+    <t>1.Verify that description with space is not added.
+2.Navigate to Sign out and click on 'Sign out'
+button.
+3.Clear test data.</t>
+  </si>
+  <si>
     <t>TC_037</t>
   </si>
   <si>
     <t>Verify that a PDF file of size less than 2 MB can be successfully uploaded.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.User is already logged in.
+2.User can access the skill sharing page.
+</t>
   </si>
   <si>
     <t>1.Click on "Add" work samples.
@@ -818,6 +1179,12 @@
     <t>The PDF file is uploaded successfully.</t>
   </si>
   <si>
+    <t>1.Verify the PDF file appears in the work samples
+2.Navigate to Sign out and click on 'Sign out'
+button.
+3.Clear test data.</t>
+  </si>
+  <si>
     <t>TC_038</t>
   </si>
   <si>
@@ -837,6 +1204,13 @@
 </t>
   </si>
   <si>
+    <t>1.Verify the PNG file appears in the work
+ samples.
+2.Navigate to Sign out and click on 'Sign out'
+button.
+3.Clear test data.</t>
+  </si>
+  <si>
     <t>TC_039</t>
   </si>
   <si>
@@ -855,6 +1229,13 @@
     <t>The TXT file is uploaded successfully.</t>
   </si>
   <si>
+    <t>1.Verify the TXT file appears in the work
+samples.
+2.Navigate to Sign out and click on 'Sign out'
+button.
+3.Clear test data.</t>
+  </si>
+  <si>
     <t>TC_040</t>
   </si>
   <si>
@@ -875,6 +1256,13 @@
     <t>The upload fails and an error message is 
 displayed indicating the file exceeds the size
 limit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Verify that file larger that 2MB is not addes.
+2.Navigate to Sign out and click on 'Sign out'
+button.
+3.Clear test data.
+</t>
   </si>
   <si>
     <t>TC_041</t>
@@ -900,6 +1288,13 @@
 supported.</t>
   </si>
   <si>
+    <t xml:space="preserve">1.Verify that unsupported files are not added.
+2.Navigate to Sign out and click on 'Sign out'
+button.
+3.Clear test data.
+</t>
+  </si>
+  <si>
     <t>TC_042</t>
   </si>
   <si>
@@ -917,13 +1312,79 @@
   </si>
   <si>
     <t>The 'Upload' button is unavailable to click.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Verify that "upload" button is unavailable.
+2.Navigate to Sign out and click on 'Sign out'
+button.
+3.Clear test data.
+</t>
+  </si>
+  <si>
+    <t>TC_043</t>
+  </si>
+  <si>
+    <t>Verify that the system can gracefully handle large payload when adding a
+language.</t>
+  </si>
+  <si>
+    <t>1.Navigate to the languages section.
+2.Delete all existing languages.</t>
+  </si>
+  <si>
+    <t>1.Click on "Add New".
+2.Enter language with a very large name(eg.,Englishhhhhhhhh etc)
+and choose language level.
+3.Click "Add"</t>
+  </si>
+  <si>
+    <t>The system should handle the large payload
+gracefully by showing an error message and 
+doesn't crash.</t>
+  </si>
+  <si>
+    <t>The system handles the large payload 
+gracefully by showing an error message 
+ie.,undefined and it doesn't crash.</t>
+  </si>
+  <si>
+    <t>1.Navigate to Sign out and click on 'Sign out'
+button.
+2.Clear test data.
+3.Verify that error message is displayed.</t>
+  </si>
+  <si>
+    <t>TC_044</t>
+  </si>
+  <si>
+    <t>Verify that the system can gracefully handle large payload when adding a
+skill.</t>
+  </si>
+  <si>
+    <t>1.Navigate to the skills section.
+2.Delete all existing skills.</t>
+  </si>
+  <si>
+    <t>1.Click on "Add New".
+2.Enter skill with a very large name(eg.,Testinggggggggggggg etc)
+and choose skill level.
+3.Click "Add"</t>
+  </si>
+  <si>
+    <t>The system should handle the large payload
+gracefully by showing an error message and 
+doesn't crash.</t>
+  </si>
+  <si>
+    <t>The system did not show an error message
+and the skill name with long text is added.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -950,6 +1411,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="6">
@@ -990,7 +1455,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1020,6 +1485,9 @@
     </xf>
     <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1238,9 +1706,11 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="61.75"/>
-    <col customWidth="1" min="3" max="3" width="55.88"/>
-    <col customWidth="1" min="4" max="4" width="36.63"/>
-    <col customWidth="1" min="5" max="5" width="35.0"/>
+    <col customWidth="1" min="3" max="3" width="44.5"/>
+    <col customWidth="1" min="4" max="4" width="55.88"/>
+    <col customWidth="1" min="5" max="5" width="36.63"/>
+    <col customWidth="1" min="6" max="6" width="35.0"/>
+    <col customWidth="1" min="8" max="8" width="36.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1262,847 +1732,1159 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>11</v>
+        <v>34</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>11</v>
+        <v>41</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>11</v>
+        <v>48</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>11</v>
+        <v>55</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>11</v>
+        <v>62</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>50</v>
+        <v>67</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>11</v>
+        <v>69</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>11</v>
+        <v>76</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>11</v>
+        <v>83</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>64</v>
+        <v>87</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>11</v>
+        <v>90</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>11</v>
+        <v>97</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>11</v>
+        <v>103</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>11</v>
+        <v>110</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>11</v>
+        <v>117</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>11</v>
+        <v>124</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>11</v>
+        <v>131</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>97</v>
+        <v>134</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>98</v>
+        <v>135</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>11</v>
+        <v>137</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>105</v>
+        <v>142</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>11</v>
+        <v>143</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>110</v>
+        <v>148</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>11</v>
+        <v>149</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>113</v>
+        <v>153</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>115</v>
+        <v>155</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>11</v>
+        <v>156</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>117</v>
+        <v>159</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>118</v>
+        <v>160</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>119</v>
+        <v>161</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>11</v>
+        <v>163</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>122</v>
+        <v>166</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>123</v>
+        <v>167</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>124</v>
+        <v>168</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>125</v>
+        <v>169</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>11</v>
+        <v>170</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>127</v>
+        <v>173</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>129</v>
+        <v>175</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>130</v>
+        <v>176</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>11</v>
+        <v>177</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>132</v>
+        <v>180</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>133</v>
+        <v>181</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>134</v>
+        <v>182</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>135</v>
+        <v>183</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>11</v>
+        <v>184</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>137</v>
+        <v>187</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>138</v>
+        <v>188</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>139</v>
+        <v>189</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>140</v>
+        <v>190</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>142</v>
+        <v>191</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>145</v>
+        <v>32</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>146</v>
+        <v>196</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>142</v>
+        <v>197</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>148</v>
+        <v>199</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>149</v>
+        <v>200</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>146</v>
+        <v>202</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>142</v>
+        <v>197</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>152</v>
+        <v>204</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>153</v>
+        <v>205</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>154</v>
+        <v>206</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>155</v>
+        <v>207</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>142</v>
+        <v>208</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>157</v>
+        <v>210</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>158</v>
+        <v>211</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>159</v>
+        <v>212</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>160</v>
+        <v>213</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>11</v>
+        <v>214</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>162</v>
+        <v>217</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>163</v>
+        <v>218</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>164</v>
+        <v>219</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>165</v>
+        <v>220</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>11</v>
+        <v>221</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>167</v>
+        <v>224</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>168</v>
+        <v>225</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>169</v>
+        <v>226</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>170</v>
+        <v>227</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>11</v>
+        <v>228</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>172</v>
+        <v>231</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>173</v>
+        <v>232</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>175</v>
+        <v>226</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>233</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>11</v>
+        <v>234</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>177</v>
+        <v>237</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>178</v>
+        <v>238</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>11</v>
+        <v>241</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>182</v>
+        <v>244</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>183</v>
+        <v>245</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>184</v>
+        <v>226</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>185</v>
+        <v>246</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>11</v>
+        <v>247</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>187</v>
+        <v>250</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>188</v>
+        <v>251</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>189</v>
+        <v>252</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>190</v>
+        <v>253</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>11</v>
+        <v>254</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>192</v>
+        <v>257</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>193</v>
+        <v>258</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>194</v>
+        <v>239</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>195</v>
+        <v>259</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>11</v>
+        <v>260</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>197</v>
+        <v>263</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>198</v>
+        <v>264</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>199</v>
+        <v>239</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>200</v>
+        <v>265</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>11</v>
+        <v>266</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>202</v>
+        <v>269</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>203</v>
+        <v>270</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>204</v>
+        <v>239</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>205</v>
+        <v>271</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>11</v>
+        <v>272</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>207</v>
+        <v>275</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>208</v>
+        <v>276</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>209</v>
+        <v>239</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>210</v>
+        <v>277</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>11</v>
+        <v>278</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>212</v>
+        <v>281</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>213</v>
+        <v>282</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>214</v>
+        <v>239</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>215</v>
+        <v>283</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>11</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>